<commit_message>
Mais uma coluna na tabela pedidos
O microsserviço Antifraude da turma 3E vai usar uma coluna extra na tabela de pedidos: 
ped_sem_pgto, tipo boolean
</commit_message>
<xml_diff>
--- a/BD_Loja_Natalia_Versao3.xlsx
+++ b/BD_Loja_Natalia_Versao3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://institutogerminare-my.sharepoint.com/personal/myrna_kagohara_germinare_org_br/Documents/Documentos/_Sistema Orientado Mensagens - 3o ano/LOJA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="220" documentId="8_{3C2DC8EF-7C48-49EB-8BAD-504A44EC32ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5B64B88-C81F-49FA-9F6A-75AE171F4037}"/>
+  <xr:revisionPtr revIDLastSave="241" documentId="8_{3C2DC8EF-7C48-49EB-8BAD-504A44EC32ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36179A58-1EB3-4A80-A479-5816B2A76685}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{94025611-3570-4B45-89FC-52385671A3EF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{94025611-3570-4B45-89FC-52385671A3EF}"/>
   </bookViews>
   <sheets>
     <sheet name="clientes" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="70">
   <si>
     <t>Descrição</t>
   </si>
@@ -244,13 +244,19 @@
   </si>
   <si>
     <t>ID do pedido. Chave primária.</t>
+  </si>
+  <si>
+    <t>ped_sem_pgto</t>
+  </si>
+  <si>
+    <t>Pedido não pago (problema de pagamento) – coluna a ser usada pelo antifraude</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -275,6 +281,19 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -327,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -338,10 +357,19 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,7 +690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ACEA923-3653-4E47-8F97-D583C84F5397}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -802,18 +830,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.90625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.1796875" style="8" customWidth="1"/>
-    <col min="3" max="4" width="41.36328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1796875" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.7265625" style="8"/>
+    <col min="1" max="1" width="29.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1796875" customWidth="1"/>
+    <col min="3" max="4" width="41.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="9" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="8" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -902,10 +929,10 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B9" s="10"/>
+      <c r="B9" s="9"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B10" s="10"/>
+      <c r="B10" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -917,124 +944,130 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF198BDC-F75A-492E-9D6A-F6CC0A4FEF15}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.90625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.1796875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="37" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" style="8"/>
-    <col min="5" max="5" width="10.7265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7265625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="14" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="8"/>
+    <col min="1" max="1" width="29.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1796875" customWidth="1"/>
+    <col min="3" max="3" width="37" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7265625" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="9" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="8" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="11" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="11" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="11" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>64</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="11" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="11" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="11" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="11" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="11" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B10" s="10"/>
+    <row r="10" spans="1:3" ht="26.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1052,15 +1085,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.6328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.1796875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="47.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.6328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.36328125" style="8" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="8"/>
+    <col min="1" max="1" width="29.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1796875" customWidth="1"/>
+    <col min="3" max="3" width="47.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="9" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="8" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1071,7 +1103,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="11" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
@@ -1082,7 +1114,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="11" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
@@ -1093,7 +1125,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="11" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
@@ -1104,7 +1136,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="11" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
@@ -1116,19 +1148,19 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B6" s="10"/>
+      <c r="B6" s="9"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B7" s="10"/>
+      <c r="B7" s="9"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B8" s="10"/>
+      <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B9" s="10"/>
+      <c r="B9" s="9"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B10" s="10"/>
+      <c r="B10" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Ajuste de chaves primárias
A tabela 'pedidos' agora tem chave primária composta: id_ped, cpf_cli, id_car_ped.
A tabela 'carrinhos' agora tem chave primária composta: id_car, prod_car.
</commit_message>
<xml_diff>
--- a/BD_Loja_Natalia_Versao3.xlsx
+++ b/BD_Loja_Natalia_Versao3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://institutogerminare-my.sharepoint.com/personal/myrna_kagohara_germinare_org_br/Documents/Documentos/_Sistema Orientado Mensagens - 3o ano/LOJA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="241" documentId="8_{3C2DC8EF-7C48-49EB-8BAD-504A44EC32ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36179A58-1EB3-4A80-A479-5816B2A76685}"/>
+  <xr:revisionPtr revIDLastSave="248" documentId="8_{3C2DC8EF-7C48-49EB-8BAD-504A44EC32ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9E6707A-F11A-4EC0-863E-5DDD44C5343C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{94025611-3570-4B45-89FC-52385671A3EF}"/>
   </bookViews>
@@ -256,7 +256,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -694,7 +694,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="29.90625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.1796875" customWidth="1"/>
@@ -704,7 +704,7 @@
     <col min="9" max="9" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="15.5">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -715,7 +715,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>47</v>
       </c>
@@ -726,7 +726,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -737,7 +737,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
@@ -748,7 +748,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -759,7 +759,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3">
       <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
@@ -770,7 +770,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3">
       <c r="A7" s="4" t="s">
         <v>20</v>
       </c>
@@ -781,7 +781,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3">
       <c r="A8" s="4" t="s">
         <v>21</v>
       </c>
@@ -792,7 +792,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3">
       <c r="A9" s="4" t="s">
         <v>48</v>
       </c>
@@ -803,7 +803,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="26.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="26.5">
       <c r="A10" s="4" t="s">
         <v>49</v>
       </c>
@@ -825,10 +825,10 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="29.90625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.1796875" customWidth="1"/>
@@ -840,7 +840,7 @@
     <col min="9" max="9" width="14.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="8" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="8" customFormat="1" ht="15.5">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -851,7 +851,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -862,7 +862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -873,7 +873,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -884,7 +884,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3">
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
@@ -895,7 +895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
@@ -906,7 +906,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
@@ -917,7 +917,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3">
       <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
@@ -928,10 +928,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3">
       <c r="B9" s="9"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3">
       <c r="B10" s="9"/>
     </row>
   </sheetData>
@@ -945,10 +945,10 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="29.90625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.1796875" customWidth="1"/>
@@ -959,7 +959,7 @@
     <col min="8" max="8" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="8" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="8" customFormat="1" ht="15.5">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -970,7 +970,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" s="10" customFormat="1" ht="13">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -981,7 +981,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" s="10" customFormat="1" ht="13">
       <c r="A3" s="4" t="s">
         <v>32</v>
       </c>
@@ -992,8 +992,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:3" s="10" customFormat="1" ht="13">
+      <c r="A4" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -1003,8 +1003,8 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:3" s="10" customFormat="1" ht="13">
+      <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -1014,7 +1014,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" s="10" customFormat="1" ht="13">
       <c r="A6" s="4" t="s">
         <v>34</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" s="10" customFormat="1" ht="13">
       <c r="A7" s="4" t="s">
         <v>35</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" s="10" customFormat="1" ht="13">
       <c r="A8" s="4" t="s">
         <v>36</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" s="10" customFormat="1" ht="13">
       <c r="A9" s="4" t="s">
         <v>37</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="26.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="26.5">
       <c r="A10" s="11" t="s">
         <v>68</v>
       </c>
@@ -1080,10 +1080,10 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="29.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.1796875" customWidth="1"/>
@@ -1092,7 +1092,7 @@
     <col min="5" max="5" width="13.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="8" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="8" customFormat="1" ht="15.5">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" s="10" customFormat="1" ht="13">
       <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
@@ -1114,8 +1114,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:3" s="10" customFormat="1" ht="13">
+      <c r="A3" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1125,7 +1125,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" s="10" customFormat="1" ht="13">
       <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" s="10" customFormat="1" ht="13">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
@@ -1147,19 +1147,19 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3">
       <c r="B6" s="9"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3">
       <c r="B7" s="9"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3">
       <c r="B8" s="9"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3">
       <c r="B9" s="9"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3">
       <c r="B10" s="9"/>
     </row>
   </sheetData>

</xml_diff>